<commit_message>
Started adding Example 3
</commit_message>
<xml_diff>
--- a/Ex1_NucleiSegmentation/ExampleResults/Ex1_NucleiSegmentation.xlsx
+++ b/Ex1_NucleiSegmentation/ExampleResults/Ex1_NucleiSegmentation.xlsx
@@ -5155,7 +5155,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.2.9</t>
+          <t>1.4.1-SNAPSHOT</t>
         </is>
       </c>
     </row>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>x86_64</t>
+          <t>aarch64</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10.16</t>
+          <t>13.5.2</t>
         </is>
       </c>
     </row>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-08-02_10-59-28</t>
+          <t>2023-09-13_21-57-05</t>
         </is>
       </c>
     </row>
@@ -5229,14 +5229,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;ROOT MIA_VERSION="1.2.9"&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.InputControl" DISABLEABLE="false" ENABLED="true" ID="1636961347222" NAME="Input control" NICKNAME="Input control" NOTES="In &amp;quot;Input control&amp;quot; we specify the path to the file we wish to work on.  At this point, no images are actually being loaded into the workspace.  We will load the images in during the main part of the workflow, typically using the &amp;quot;Load image&amp;quot; module.  These can be inserted anywhere in the workflow, meaning we're not wasting memory by opening them before they're needed.&amp;#10;&amp;#10;Here, we can specify a single file or, if we wish to run in batch mode, a folder.  When dealing with folders we may not want to load all the files contained within.  Therefore, it's possible to add filters that will help us process only the images of interest.  In the example here, we've got it set to only load files with .tif extensions and to skip anything with &amp;quot;_overlay&amp;quot; in the name (these will be created by this workflow).&amp;#10;&amp;#10;In MIA, parameters can be made visible for users working in &amp;quot;Processing view&amp;quot; by clicking the button to the right of the parameter.  In this workflow, the &amp;quot;Input path&amp;quot; is one such visible parameter." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input path" NICKNAME="Input path" VALUE="/Users/sc13967/Documents/Programming/Java/mia-examples/Ex1_NucleiSegmentation" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="All series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series list" NICKNAME="Series list" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first file per folder" NICKNAME="Only load first file per folder" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first matching group" NICKNAME="Only load first matching group" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pattern" NICKNAME="Pattern" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Spatial unit" NICKNAME="Spatial unit" VALUE="Micrometres" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Temporal unit" NICKNAME="Temporal unit" VALUE="Milliseconds" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Ignore case" NICKNAME="Ignore case" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filter" NICKNAME="Add filter" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Extension" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="tif" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (include)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Filename" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (exclude)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;/COLLECTION&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Simultaneous jobs" NICKNAME="Simultaneous jobs" VALUE="1" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Extension" NICKNAME="Extension"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="File" NICKNAME="File"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filename" NICKNAME="Filename"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filepath" NICKNAME="Filepath"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Series name" NICKNAME="Series name"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Series number" NICKNAME="Series number"/&gt;&lt;/METADATA&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.OutputControl" DISABLEABLE="false" ENABLED="true" ID="1636961347222" NAME="Output control" NICKNAME="Output control" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Add variable" NICKNAME="Add variable" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION/&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Run macro" NICKNAME="Run macro" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro mode" NICKNAME="Macro mode" VALUE="Macro text" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro text" NICKNAME="Macro text" VALUE="run(&amp;quot;Enable MIA Extensions&amp;quot;);&amp;#10;&amp;#10;// Get a list of Workspace IDs with Ext.MIA_GetListOfWorkspaceIDs() and set active workspace with Ext.MIA_SetActiveWorkspace(ID)." VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro file" NICKNAME="Macro file" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export mode" NICKNAME="Export mode" VALUE="All together" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Individual save location" NICKNAME="Individual save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Group save location" NICKNAME="Group save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file/folder name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for grouping" NICKNAME="Metadata item for grouping" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Continuous data export" NICKNAME="Continuous data export" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save every n files" NICKNAME="Save every n files" VALUE="10" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export summary" NICKNAME="Export summary" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Summary mode" NICKNAME="Summary mode" VALUE="Per input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for summary" NICKNAME="Metadata item for summary" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Show object counts" NICKNAME="Show object counts" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export individual objects" NICKNAME="Export individual objects" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962470785" NAME="GUI separator" NICKNAME="File loading" NOTES="These separators have no direct effect on the workflow.  Instead, they're simply to help visually break the workflow down into easy-to-understand sections.  &amp;#10;&amp;#10;Clicking the power icon to the left of the separator will disable all modules contained within this section.&amp;#10;&amp;#10;Sections can also be collapsed/expanded by clicking the arrows to the left or right of the separator name.  When collapsed, all modules will still be run." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageLoader" DISABLEABLE="false" ENABLED="true" ID="1636961348488" NAME="Load image" NICKNAME="Load image" NOTES="&amp;quot;Load image&amp;quot; is the main module for loading images from file into the workspace.  In most cases, this will be from the &amp;quot;Current file&amp;quot; (i.e. the one selected in &amp;quot;Input control&amp;quot;); however, it is possible to use metadata values to load other images, although this will be covered in a later example.&amp;#10;&amp;#10;For multi-dimensional images it's possible to load of subset of channels, slices or timepoints.  This way we don't need to load the entire image into the computer's memory - something that can be very useful when dealing with largeimage stacks.  For example, we may only want the first channel or a particular subset of slices.&amp;#10;&amp;#10;In this example, &amp;quot;Channels&amp;quot;, &amp;quot;Slices&amp;quot; and &amp;quot;Frames&amp;quot; are all set to &amp;quot;1-end&amp;quot;, which will load every available image; however, subsets can be selected using ranges (e.g. &amp;quot;4-7&amp;quot;), comma-separated lists (e.g. &amp;quot;1,5,6,7&amp;quot;).&amp;#10;&amp;#10;Multiple &amp;quot;Load image&amp;quot; modules can be inserted into the workflow as and when they are required.  This also allows us to manage the memory being used at any time.&amp;#10;&amp;#10;This module will add an image called &amp;quot;Raw&amp;quot; to the workspace.  The image will then be accessible by all subsequent modules.  Although not done in this example workflow, images can be assigned measurement values.  Measurements can be exported to the final Excel file or used by subsequent modules." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Import mode" NICKNAME="Import mode" VALUE="Current file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reader" NICKNAME="Reader" VALUE="Bio-Formats" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Sequence root name" NICKNAME="Sequence root name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Name format" NICKNAME="Name format" VALUE="Generic (from metadata)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Comment" NICKNAME="Comment" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Extension" NICKNAME="Extension" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Generic format" NICKNAME="Generic format" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Include series number" NICKNAME="Include series number" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="Current series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series number" NICKNAME="Series number" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channels" NICKNAME="Channels" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Slices" NICKNAME="Slices" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frames" NICKNAME="Frames" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel" NICKNAME="Channel" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Crop mode" NICKNAME="Crop mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image" NICKNAME="Reference image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Left coordinate" NICKNAME="Left coordinate" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Top coordinate" NICKNAME="Top coordinate" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Width" NICKNAME="Width" VALUE="512" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Height" NICKNAME="Height" VALUE="512" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Objects for limits" NICKNAME="Objects for limits" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Scale mode" NICKNAME="Scale mode" VALUE="No scaling" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X scale factor" NICKNAME="X scale factor" VALUE="0.75" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y scale factor" NICKNAME="Y scale factor" VALUE="0.75" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Dimension mismatch mode" NICKNAME="Dimension mismatch mode" VALUE="Disallow (fail upon mismatch)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pad intensity mode" NICKNAME="Pad intensity mode" VALUE="Black (0)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual spatial calibration" NICKNAME="Set manual spatial calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="XY calibration (dist/px)" NICKNAME="XY calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z calibration (dist/px)" NICKNAME="Z calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual temporal calibration" NICKNAME="Set manual temporal calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame interval (time/frame)" NICKNAME="Frame interval (time/frame)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Force bit depth" NICKNAME="Force bit depth" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output bit depth" NICKNAME="Output bit depth" VALUE="8" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum input intensity" NICKNAME="Minimum input intensity" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum input intensity" NICKNAME="Maximum input intensity" VALUE="1.0" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962481633" NAME="GUI separator" NICKNAME="Segmentation" NOTES="The modules in this section deal with segmentation of the nuclei in 3D." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.FilterImage" DISABLEABLE="false" ENABLED="true" ID="1636961810491" NAME="Filter image" NICKNAME="Filter image" NOTES="Taking the &amp;quot;Raw&amp;quot; image we loaded earlier in the workflow we apply a 2D median filter to each slice.&amp;#10;&amp;#10;The filtered image will be added to the workspace with the name &amp;quot;Binary&amp;quot;.  While this isn't a binarised image just yet, MIA allows us to change images in the workspace, thus avoiding wasting memory on intermediate images we no longer need." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Median 2D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter radius" NICKNAME="Filter radius" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calibrated units" NICKNAME="Calibrated units" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Rolling filter method" NICKNAME="Rolling filter method" VALUE="Average" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Window indices" NICKNAME="Window indices" VALUE="-1-1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Contour contrast" NICKNAME="Contour contrast" VALUE="Dark line" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.transform.ProjectImage" DISABLEABLE="false" ENABLED="true" ID="1636961855499" NAME="Project image" NICKNAME="Project image" NOTES="For the purpose of background subtraction we will create a minimum intensity Z-axis projection and subtract this from all slices (subtraction will be done in the next module).&amp;#10;&amp;#10;This module outputs the projected image (which is now a single slice) to the workspace as &amp;quot;MinProjection&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="MinProjection" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Projection axis" NICKNAME="Projection axis" VALUE="Z" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Projection mode" NICKNAME="Projection mode" VALUE="Minimum" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.ImageCalculator" DISABLEABLE="false" ENABLED="true" ID="1636961888899" NAME="Image calculator" NICKNAME="Image calculator" NOTES="Subtracting the minimum intensity projection image from each slice of the &amp;quot;Binary&amp;quot; image.&amp;#10;&amp;#10;In this instance, &amp;quot;Input image 1&amp;quot; is a Z-stack and &amp;quot;Input image 2&amp;quot; is a single slice.  As such, the single slice will be subtracted from each slice of &amp;quot;Binary&amp;quot;.  If we had provided two Z-stacks of equal dimensions, the corresponding slices would have been subtracted (i.e. slice 5 subtracted from slice 5).&amp;#10;&amp;#10;Rather than create a new, background-subtracted image, the image stored in the workspace as &amp;quot;Binary&amp;quot; will be updated.  This prevents us unnecessarily creating new images and keeps the list of available images tidier." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image 1" NICKNAME="Input image 1" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image 2" NICKNAME="Input image 2" VALUE="MinProjection" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Overwrite mode" NICKNAME="Overwrite mode" VALUE="Overwrite image 1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output 32-bit image" NICKNAME="Output 32-bit image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calculation method" NICKNAME="Calculation method" VALUE="Subtract image 2 from image 1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Image 2 relative contribution" NICKNAME="Image 2 relative contribution" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set NaN values to zero" NICKNAME="Set NaN values to zero" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.threshold.GlobalAutoThreshold" DISABLEABLE="false" ENABLED="true" ID="1636961828208" NAME="Global auto-threshold" NICKNAME="Global auto-threshold" NOTES="Now binarising the filtered and background-subtracted image called &amp;quot;Binary&amp;quot;.&amp;#10;&amp;#10;As with the &amp;quot;Image calculator&amp;quot; module, we apply the changes from this module to the input image rather than storing them as a new image in the workspace.&amp;#10;&amp;#10;Modules dealing with binary images typically have the &amp;quot;Binary logic&amp;quot; control.  This determines whether objects are considered as white objects on a black background or as black objects on a white background.  In both cases, &amp;quot;black&amp;quot; corresponds to 0-intensity and &amp;quot;white&amp;quot; corresponds to 255 (irrespective of applied LUT)." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output mode" NICKNAME="Output mode" VALUE="Calculate and apply" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Algorithm" NICKNAME="Algorithm" VALUE="Huang" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Threshold multiplier" NICKNAME="Threshold multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use lower threshold limit" NICKNAME="Use lower threshold limit" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Lower threshold limit" NICKNAME="Lower threshold limit" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure on objects" NICKNAME="Measure on objects" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" IMAGE_NAME="Binary" NAME="THRESHOLD // GLOBAL Huang" NICKNAME="THRESHOLD // GLOBAL Huang"/&gt;&lt;/IMAGE_MEASUREMENTS&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.binary.FillHoles" DISABLEABLE="false" ENABLED="true" ID="1636961945985" NAME="Fill holes" NICKNAME="Fill holes" NOTES="Performing a 3D fill holes operation on the binarised image.&amp;#10;&amp;#10;This module uses of the MorphoLibJ implementation of binary hole filling." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.binary.Watershed" DISABLEABLE="false" ENABLED="true" ID="1636961976414" NAME="Watershed transform" NICKNAME="Watershed transform" NOTES="Performing watershed segmentation to split adjacent nuclei which have become merged during filtering and binarisation.  &amp;#10;&amp;#10;This module uses of the MorphoLibJ implementation of watershed, wlhich allows us to optionally specify markers and the dynamic value (how aggressively regions are split down)." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use markers" NICKNAME="Use markers" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input marker image" NICKNAME="Input marker image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Intensity mode" NICKNAME="Intensity mode" VALUE="Distance" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Intensity image" NICKNAME="Intensity image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Dynamic" NICKNAME="Dynamic" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Match Z to XY" NICKNAME="Match Z to XY" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.detect.IdentifyObjects" DISABLEABLE="false" ENABLED="true" ID="1636962210444" NAME="Identify objects" NICKNAME="Identify objects" NOTES="Using connected components labelling to identify the nuclei as contiguous regions of &amp;quot;foreground&amp;quot; pixels (defined by the &amp;quot;Binary logic&amp;quot; parameter).&amp;#10;&amp;#10;This module takes an image from the workspace, but outputs a collection of objects.  Objects are stored as individual entities within the output collection.  Each object has its own set of coordinates and can be assigned relationships (to other objects) and measurements.&amp;#10;&amp;#10;Object coordinates can be stored using three different systems (Pointlist, Quadtree and Octree), each of which has uinque memory usage characterisics.  Other than memory usage, there should be no difference in between the systems.  Here we'll use &amp;quot;Quadtree&amp;quot; as it's generally more efficient for solid objects.  More information on these is provided at https://mianalysis.github.io.  " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output objects" NICKNAME="Output objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Detection mode" NICKNAME="Detection mode" VALUE="3D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Identify as single object" NICKNAME="Identify as single object" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Volume type" NICKNAME="Volume type" VALUE="Quadtree" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum strip width (px)" NICKNAME="Minimum strip width (px)" VALUE="60" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.spatial.MeasureObjectShape" DISABLEABLE="false" ENABLED="true" ID="1636962319317" NAME="Measure object shape" NICKNAME="Measure object shape" NOTES="Calculating the volume of each object stored in the &amp;quot;Nuclei&amp;quot; collection.&amp;#10;&amp;#10;As with the image processing modules earlier in this workflow, the &amp;quot;Measure object shape&amp;quot; module can take any previously-generated objects as inputs.&amp;#10;&amp;#10;The selected measurements are calculated for each object in the &amp;quot;Nuclei&amp;quot; collection.  These measurements are stored with the relevant object and can be used in subsequent modules." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure volume" NICKNAME="Measure volume" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected area" NICKNAME="Measure projected area" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected diameter" NICKNAME="Measure projected diameter" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected perimeter" NICKNAME="Measure projected perimeter" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure 3D metrics" NICKNAME="Measure 3D metrics" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Surface area method" NICKNAME="Surface area method" VALUE="13 directions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // BASE_AREA_(PX²)" NICKNAME="SHAPE // BASE_AREA_(PX²)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // BASE_AREA_(µm²)" NICKNAME="SHAPE // BASE_AREA_(µm²)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // HEIGHT_(SLICE)" NICKNAME="SHAPE // HEIGHT_(SLICE)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // HEIGHT_(µm)" NICKNAME="SHAPE // HEIGHT_(µm)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // N_VOXELS" NICKNAME="SHAPE // N_VOXELS" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // VOLUME_(PX³)" NICKNAME="SHAPE // VOLUME_(PX³)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // VOLUME_(µm³)" NICKNAME="SHAPE // VOLUME_(µm³)" OBJECT_NAME="Nuclei"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByMeasurement" DISABLEABLE="true" ENABLED="true" ID="1636962353494" NAME="Based on measurement" NICKNAME="Volume filter" NOTES="With volume measurements now assigned to each object in the &amp;quot;Nuclei&amp;quot; collection, we can apply a filter to remove those smaller than a specified value.&amp;#10;&amp;#10;In this module, any &amp;quot; Nuclei&amp;quot; objects less than the specified &amp;quot;Reference value&amp;quot; will simply be removed from the collection (it is also possible to add them to a new collection using the &amp;quot;Filter mode&amp;quot; control).&amp;#10;&amp;#10;This is a useful operation to be displayed in MIA's &amp;quot;Processing view&amp;quot;, so the &amp;quot;Reference value&amp;quot; parameter has been selected as editable using the toggle to its right.&amp;#10;&amp;#10;By having &amp;quot;Can be disabled&amp;quot; selected at the top of the module page, processing view will display the enable/disable control.&amp;#10;&amp;#10;Finally, this module has been renamed from &amp;quot;Based on measurement&amp;quot; to &amp;quot;Volume filter&amp;quot; as this is more intuitive as to its purpose.  Modules (and parameters) can be renamed by right-clicking on their name." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Remove filtered objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Less than" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="100" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference</t>
+          <t>&lt;?xml version="1.0" encoding="UTF-8" standalone="no"?&gt;&lt;ROOT MIA_VERSION="1.4.1-SNAPSHOT"&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.InputControl" DISABLEABLE="false" ENABLED="true" ID="1636961347222" NAME="Input control" NICKNAME="Input control" NOTES="In &amp;quot;Input control&amp;quot; we specify the path to the file we wish to work on.  At this point, no images are actually being loaded into the workspace.  We will load the images in during the main part of the workflow, typically using the &amp;quot;Load image&amp;quot; module.  These can be inserted anywhere in the workflow, meaning we're not wasting memory by opening them before they're needed.&amp;#10;&amp;#10;Here, we can specify a single file or, if we wish to run in batch mode, a folder.  When dealing with folders we may not want to load all the files contained within.  Therefore, it's possible to add filters that will help us process only the images of interest.  In the example here, we've got it set to only load files with .tif extensions and to skip anything with &amp;quot;_overlay&amp;quot; in the name (these will be created by this workflow).&amp;#10;&amp;#10;In MIA, parameters can be made visible for users working in &amp;quot;Processing view&amp;quot; by clicking the button to the right of the parameter.  In this workflow, the &amp;quot;Input path&amp;quot; is one such visible parameter." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input path" NICKNAME="Input path" VALUE="/Users/sc13967/Documents/Programming/Java/mia-examples/Ex1_NucleiSegmentation" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="All series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series list" NICKNAME="Series list" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first file per folder" NICKNAME="Only load first file per folder" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first matching group" NICKNAME="Only load first matching group" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pattern" NICKNAME="Pattern" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Spatial unit" NICKNAME="Spatial unit" VALUE="Micrometres" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Temporal unit" NICKNAME="Temporal unit" VALUE="Milliseconds" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Ignore case" NICKNAME="Ignore case" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filter" NICKNAME="Add filter" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Extension" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="tif" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (include)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Filename" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (exclude)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;/COLLECTION&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Simultaneous jobs" NICKNAME="Simultaneous jobs" VALUE="1" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Extension" NICKNAME="Extension"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="File" NICKNAME="File"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filename" NICKNAME="Filename"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filepath" NICKNAME="Filepath"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Series name" NICKNAME="Series name"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Series number" NICKNAME="Series number"/&gt;&lt;/METADATA&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.OutputControl" DISABLEABLE="false" ENABLED="true" ID="1636961347222" NAME="Output control" NICKNAME="Output control" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Add variable" NICKNAME="Add variable" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION/&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Run macro" NICKNAME="Run macro" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro mode" NICKNAME="Macro mode" VALUE="Macro text" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro text" NICKNAME="Macro text" VALUE="run(&amp;quot;Enable MIA Extensions&amp;quot;);&amp;#10;&amp;#10;// Get a list of Workspace IDs with Ext.MIA_GetListOfWorkspaceIDs() and set active workspace with Ext.MIA_SetActiveWorkspace(ID)." VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro file" NICKNAME="Macro file" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export mode" NICKNAME="Export mode" VALUE="All together" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Individual save location" NICKNAME="Individual save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Group save location" NICKNAME="Group save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file/folder name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for grouping" NICKNAME="Metadata item for grouping" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Continuous data export" NICKNAME="Continuous data export" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save every n files" NICKNAME="Save every n files" VALUE="10" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export summary" NICKNAME="Export summary" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Summary mode" NICKNAME="Summary mode" VALUE="Per input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for summary" NICKNAME="Metadata item for summary" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Show object counts" NICKNAME="Show object counts" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export individual objects" NICKNAME="Export individual objects" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962470785" NAME="GUI separator" NICKNAME="File loading" NOTES="These separators have no direct effect on the workflow.  Instead, they're simply to help visually break the workflow down into easy-to-understand sections.  &amp;#10;&amp;#10;Clicking the power icon to the left of the separator will disable all modules contained within this section.&amp;#10;&amp;#10;Sections can also be collapsed/expanded by clicking the arrows to the left or right of the separator name.  When collapsed, all modules will still be run." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageLoader" DISABLEABLE="false" ENABLED="true" ID="1636961348488" NAME="Load image" NICKNAME="Load image" NOTES="&amp;quot;Load image&amp;quot; is the main module for loading images from file into the workspace.  In most cases, this will be from the &amp;quot;Current file&amp;quot; (i.e. the one selected in &amp;quot;Input control&amp;quot;); however, it is possible to use metadata values to load other images, although this will be covered in a later example.&amp;#10;&amp;#10;For multi-dimensional images it's possible to load of subset of channels, slices or timepoints.  This way we don't need to load the entire image into the computer's memory - something that can be very useful when dealing with largeimage stacks.  For example, we may only want the first channel or a particular subset of slices.&amp;#10;&amp;#10;In this example, &amp;quot;Channels&amp;quot;, &amp;quot;Slices&amp;quot; and &amp;quot;Frames&amp;quot; are all set to &amp;quot;1-end&amp;quot;, which will load every available image; however, subsets can be selected using ranges (e.g. &amp;quot;4-7&amp;quot;), comma-separated lists (e.g. &amp;quot;1,5,6,7&amp;quot;).&amp;#10;&amp;#10;Multiple &amp;quot;Load image&amp;quot; modules can be inserted into the workflow as and when they are required.  This also allows us to manage the memory being used at any time.&amp;#10;&amp;#10;This module will add an image called &amp;quot;Raw&amp;quot; to the workspace.  The image will then be accessible by all subsequent modules.  Although not done in this example workflow, images can be assigned measurement values.  Measurements can be exported to the final Excel file or used by subsequent modules." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Import mode" NICKNAME="Import mode" VALUE="Current file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reader" NICKNAME="Reader" VALUE="Bio-Formats" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Sequence root name" NICKNAME="Sequence root name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Name format" NICKNAME="Name format" VALUE="Generic (from metadata)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Comment" NICKNAME="Comment" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Extension" NICKNAME="Extension" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Generic format" NICKNAME="Generic format" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Include series number" NICKNAME="Include series number" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="Current series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series number" NICKNAME="Series number" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channels" NICKNAME="Channels" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Slices" NICKNAME="Slices" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frames" NICKNAME="Frames" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel" NICKNAME="Channel" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Crop mode" NICKNAME="Crop mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image" NICKNAME="Reference image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Left coordinate" NICKNAME="Left coordinate" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Top coordinate" NICKNAME="Top coordinate" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Width" NICKNAME="Width" VALUE="512" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Height" NICKNAME="Height" VALUE="512" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Objects for limits" NICKNAME="Objects for limits" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Scale mode" NICKNAME="Scale mode" VALUE="No scaling" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X scale factor" NICKNAME="X scale factor" VALUE="0.75" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y scale factor" NICKNAME="Y scale factor" VALUE="0.75" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Dimension mismatch mode" NICKNAME="Dimension mismatch mode" VALUE="Disallow (fail upon mismatch)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pad intensity mode" NICKNAME="Pad intensity mode" VALUE="Black (0)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual spatial calibration" NICKNAME="Set manual spatial calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="XY calibration (dist/px)" NICKNAME="XY calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z calibration (dist/px)" NICKNAME="Z calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual temporal calibration" NICKNAME="Set manual temporal calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame interval (time/frame)" NICKNAME="Frame interval (time/frame)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Force bit depth" NICKNAME="Force bit depth" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output bit depth" NICKNAME="Output bit depth" VALUE="8" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum input intensity" NICKNAME="Minimum input intensity" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum input intensity" NICKNAME="Maximum input intensity" VALUE="1.0" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962481633" NAME="GUI separator" NICKNAME="Segmentation" NOTES="The modules in this section deal with segmentation of the nuclei in 3D." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.FilterImage" DISABLEABLE="false" ENABLED="true" ID="1636961810491" NAME="Filter image" NICKNAME="Filter image" NOTES="Taking the &amp;quot;Raw&amp;quot; image we loaded earlier in the workflow we apply a 2D median filter to each slice.&amp;#10;&amp;#10;The filtered image will be added to the workspace with the name &amp;quot;Binary&amp;quot;.  While this isn't a binarised image just yet, MIA allows us to change images in the workspace, thus avoiding wasting memory on intermediate images we no longer need." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Median 2D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter radius" NICKNAME="Filter radius" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter radius 2" NICKNAME="Filter radius 2" VALUE="3.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calibrated units" NICKNAME="Calibrated units" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Rolling filter method" NICKNAME="Rolling filter method" VALUE="Average" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Window indices" NICKNAME="Window indices" VALUE="-1-1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Contour contrast" NICKNAME="Contour contrast" VALUE="Dark line" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.transform.ProjectImage" DISABLEABLE="false" ENABLED="true" ID="1636961855499" NAME="Project image" NICKNAME="Project image" NOTES="For the purpose of background subtraction we will create a minimum intensity Z-axis projection and subtract this from all slices (subtraction will be done in the next module).&amp;#10;&amp;#10;This module outputs the projected image (which is now a single slice) to the workspace as &amp;quot;MinProjection&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="MinProjection" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Projection axis" NICKNAME="Projection axis" VALUE="Z" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Projection mode" NICKNAME="Projection mode" VALUE="Minimum" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.ImageCalculator" DISABLEABLE="false" ENABLED="true" ID="1636961888899" NAME="Image calculator" NICKNAME="Image calculator" NOTES="Subtracting the minimum intensity projection image from each slice of the &amp;quot;Binary&amp;quot; image.&amp;#10;&amp;#10;In this instance, &amp;quot;Input image 1&amp;quot; is a Z-stack and &amp;quot;Input image 2&amp;quot; is a single slice.  As such, the single slice will be subtracted from each slice of &amp;quot;Binary&amp;quot;.  If we had provided two Z-stacks of equal dimensions, the corresponding slices would have been subtracted (i.e. slice 5 subtracted from slice 5).&amp;#10;&amp;#10;Rather than create a new, background-subtracted image, the image stored in the workspace as &amp;quot;Binary&amp;quot; will be updated.  This prevents us unnecessarily creating new images and keeps the list of available images tidier." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image 1" NICKNAME="Input image 1" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image 2" NICKNAME="Input image 2" VALUE="MinProjection" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Overwrite mode" NICKNAME="Overwrite mode" VALUE="Overwrite image 1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output 32-bit image" NICKNAME="Output 32-bit image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calculation method" NICKNAME="Calculation method" VALUE="Subtract image 2 from image 1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Image 2 relative contribution" NICKNAME="Image 2 relative contribution" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set NaN values to zero" NICKNAME="Set NaN values to zero" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.threshold.GlobalAutoThreshold" DISABLEABLE="false" ENABLED="true" ID="1636961828208" NAME="Global auto-threshold" NICKNAME="Global auto-threshold" NOTES="Now binarising the filtered and background-subtracted image called &amp;quot;Binary&amp;quot;.&amp;#10;&amp;#10;As with the &amp;quot;Image calculator&amp;quot; module, we apply the changes from this module to the input image rather than storing them as a new image in the workspace.&amp;#10;&amp;#10;Modules dealing with binary images typically have the &amp;quot;Binary logic&amp;quot; control.  This determines whether objects are considered as white objects on a black background or as black objects on a white background.  In both cases, &amp;quot;black&amp;quot; corresponds to 0-intensity and &amp;quot;white&amp;quot; corresponds to 255 (irrespective of applied LUT)." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output mode" NICKNAME="Output mode" VALUE="Calculate and apply" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Algorithm" NICKNAME="Algorithm" VALUE="Huang" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Threshold multiplier" NICKNAME="Threshold multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use lower threshold limit" NICKNAME="Use lower threshold limit" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Lower threshold limit" NICKNAME="Lower threshold limit" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure on objects" NICKNAME="Measure on objects" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" IMAGE_NAME="Binary" NAME="THRESHOLD // GLOBAL Huang" NICKNAME="THRESHOLD // GLOBAL Huang"/&gt;&lt;/IMAGE_MEASUREMENTS&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.binary.FillHoles" DISABLEABLE="false" ENABLED="true" ID="1636961945985" NAME="Fill holes" NICKNAME="Fill holes" NOTES="Performing a 3D fill holes operation on the binarised image.&amp;#10;&amp;#10;This module uses of the MorphoLibJ implementation of binary hole filling." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.binary.Watershed" DISABLEABLE="false" ENABLED="true" ID="1636961976414" NAME="Watershed transform" NICKNAME="Watershed transform" NOTES="Performing watershed segmentation to split adjacent nuclei which have become merged during filtering and binarisation.  &amp;#10;&amp;#10;This module uses of the MorphoLibJ implementation of watershed, wlhich allows us to optionally specify markers and the dynamic value (how aggressively regions are split down)." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use markers" NICKNAME="Use markers" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input marker image" NICKNAME="Input marker image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Intensity mode" NICKNAME="Intensity mode" VALUE="Distance" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Intensity image" NICKNAME="Intensity image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Dynamic" NICKNAME="Dynamic" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Match Z to XY" NICKNAME="Match Z to XY" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.detect.IdentifyObjects" DISABLEABLE="false" ENABLED="true" ID="1636962210444" NAME="Identify objects" NICKNAME="Identify objects" NOTES="Using connected components labelling to identify the nuclei as contiguous regions of &amp;quot;foreground&amp;quot; pixels (defined by the &amp;quot;Binary logic&amp;quot; parameter).&amp;#10;&amp;#10;This module takes an image from the workspace, but outputs a collection of objects.  Objects are stored as individual entities within the output collection.  Each object has its own set of coordinates and can be assigned relationships (to other objects) and measurements.&amp;#10;&amp;#10;Object coordinates can be stored using three different systems (Pointlist, Quadtree and Octree), each of which has uinque memory usage characterisics.  Other than memory usage, there should be no difference in between the systems.  Here we'll use &amp;quot;Quadtree&amp;quot; as it's generally more efficient for solid objects.  More information on these is provided at https://mianalysis.github.io.  " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output objects" NICKNAME="Output objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Detection mode" NICKNAME="Detection mode" VALUE="3D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Identify as single object" NICKNAME="Identify as single object" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Volume type" NICKNAME="Volume type" VALUE="Quadtree" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum strip width (px)" NICKNAME="Minimum strip width (px)" VALUE="60" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.spatial.MeasureObjectShape" DISABLEABLE="false" ENABLED="true" ID="1636962319317" NAME="Measure object shape" NICKNAME="Measure object shape" NOTES="Calculating the volume of each object stored in the &amp;quot;Nuclei&amp;quot; collection.&amp;#10;&amp;#10;As with the image processing modules earlier in this workflow, the &amp;quot;Measure object shape&amp;quot; module can take any previously-generated objects as inputs.&amp;#10;&amp;#10;The selected measurements are calculated for each object in the &amp;quot;Nuclei&amp;quot; collection.  These measurements are stored with the relevant object and can be used in subsequent modules." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure volume" NICKNAME="Measure volume" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected area" NICKNAME="Measure projected area" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected diameter" NICKNAME="Measure projected diameter" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected perimeter" NICKNAME="Measure projected perimeter" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure 3D metrics" NICKNAME="Measure 3D metrics" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Surface area method" NICKNAME="Surface area method" VALUE="13 directions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // BASE_AREA_(PX²)" NICKNAME="SHAPE // BASE_AREA_(PX²)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // BASE_AREA_(µm²)" NICKNAME="SHAPE // BASE_AREA_(µm²)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // HEIGHT_(SLICE)" NICKNAME="SHAPE // HEIGHT_(SLICE)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // HEIGHT_(µm)" NICKNAME="SHAPE // HEIGHT_(µm)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // N_VOXELS" NICKNAME="SHAPE // N_VOXELS" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // VOLUME_(PX³)" NICKNAME="SHAPE // VOLUME_(PX³)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // VOLUME_(µm³)" NICKNAME="SHAPE // VOLUME_(µm³)" OBJECT_NAME="Nuclei"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByMeasurement" DISABLEABLE="true" ENABLED="true" ID="1636962353494" NAME="Based on measurement" NICKNAME="Volume filter" NOTES="With volume measurements now assigned to each object in the &amp;quot;Nuclei&amp;quot; collection, we can apply a filter to remove those smaller than a specified value.&amp;#10;&amp;#10;In this module, any &amp;quot; Nuclei&amp;quot; objects less than the specified &amp;quot;Reference value&amp;quot; will simply be removed from the collection (it is also possible to add them to a new collection using the &amp;quot;Filter mode&amp;quot; control).&amp;#10;&amp;#10;This is a useful operation to be displayed in MIA's &amp;quot;Processing view&amp;quot;, so the &amp;quot;Reference value&amp;quot; parameter has been selected as editable using the toggle to its right.&amp;#10;&amp;#10;By having &amp;quot;Can be disabled&amp;quot; selected at the top of the module page, processing view will display the enable/disable control.&amp;#10;&amp;#10;Finally, this module has been renamed from &amp;quot;Based on measurement&amp;quot; to &amp;quot;Volume filter&amp;quot; as this is more intuitive as to its purpose.  Modules (and parameters) can be renamed by right-clicking on their name." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Remove filtered objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Less than" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="100" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement to filter on" NICKNAME="Measurement to filter on" VALUE="SHAPE // VOLUME_(µm³)" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962497111" NAME="GUI separator" NICKNAME="Measurements" NOTES="Modules in this section are involved with additional measurements assigned to the detectetd nuclei." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.intensity.MeasureObjectIntensity" DISABLEABLE="false" ENABLED="true" ID="1636962461046" NAME="Measure object intensity" NICKNAME="Measure object intensity" NOTES="Measuring the intensity of the &amp;quot;Raw&amp;quot; image coincident with each &amp;quot;Nuclei&amp;quot; object.&amp;#10;&amp;#10;As with the &amp;quot;Measure object shape&amp;quot; module, this will make a separate measurement for each object in the collection.  In this case that measurement is the mean, min, max, sum and standard deviation of all pixel intensities coincident with the coordinates of each object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure weighted centre" NICKNAME="Measure weighted centre" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_MAX" NICKNAME="INTENSITY // Raw_MAX" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_MEAN" NICKNAME="INTENSITY // Raw_MEAN" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_MIN" NICKNAME="INTENSITY // Raw_MIN" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_STDEV" NICKNAME="INTENSITY // Raw_STDEV" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_SUM" NICKNAME="INTENSITY // Raw_SUM" OBJECT_NAME="Nuclei"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.process.FitLongestChord" DISABLEABLE="false" ENABLED="true" ID="1690970094383" NAME="Fit longest chord" NICKNAME="Fit longest chord" NOTES="Measuring the &amp;quot;longest chord&amp;quot; for each nucleus.  The longest chord is the longest straight line that can be placed between any two points on the surface of an object.  In other words, it is the maximum diameter." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure object width" NICKNAME="Measure object width" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure object orientation" NICKNAME="Measure object orientation" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store end points" NICKNAME="Store end points" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="LONGEST_CHORD // LENGTH (PX)" NICKNAME="LONGEST_CHORD // LENGTH (PX)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="LONGEST_CHORD // LENGTH (µm)" NICKNAME="LONGEST_CHORD // LENGTH (µm)" OBJECT_NAME="Nuclei"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962505950" NAME="GUI separator" NICKNAME="Image output" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectFill" DISABLEABLE="false" ENABLED="true" ID="1636962635839" NAME="Add object fill" NICKNAME="Add object fill" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Measurement value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="White" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="LONGEST_CHORD // LENGTH (µm)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="25" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectOutline" DISABLEABLE="false" ENABLED="true" ID="1636962596250" NAME="Add object outline" NICKNAME="Add object outline" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="White" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reduce line complexity" NICKNAME="Reduce line complexity" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Line interpolation" NICKNAME="Line interpolation" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Line width" NICKNAME="Line width" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddLabels" DISABLEABLE="false" ENABLED="true" ID="1690970140097" NAME="Add labels" NICKNAME="Add labels" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="White" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Label mode" NICKNAME="Label mode" VALUE="ID" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Decimal places" NICKNAME="Decimal places" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use scientific notation" NICKNAME="Use scientific notation" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Label size" NICKNAME="Label size" VALUE="10" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X-offset" NICKNAME="X-offset" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y-offset" NICKNAME="Y-offset" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Centre text" NICKNAME="Centre text" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for label" NICKNAME="Child objects for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for label" NICKNAME="Parent object for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for label" NICKNAME="Partner objects for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for label" NICKNAME="Measurement for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Prefix" NICKNAME="Prefix" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Suffix" NICKNAME="Suffix" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Label position" NICKNAME="Label position" VALUE="Centre of object" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X-position measurement" NICKNAME="X-position measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y-position measurement" NICKNAME="Y-position measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z-position measurement" NICKNAME="Z-position measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X-position" NICKNAME="X-position" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y-position" NICKNAME="Y-position" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z-position" NICKNAME="Z-position" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all object slices" NICKNAME="Render in all object slices" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.ShowImage" DISABLEABLE="true" ENABLED="false" ID="1636962716078" NAME="Show image" NICKNAME="Show image" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="true"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Display image" NICKNAME="Display image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Title mode" NICKNAME="Title mode" VALUE="Image name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quick normalisation" NICKNAME="Quick normalisation" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageSaver" DISABLEABLE="false" ENABLED="true" ID="1636962735245" NAME="Save image" NICKNAME="Save image" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Save location" NICKNAME="Save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name (generic)" NICKNAME="File name (generic)" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append series mode" NICKNAME="Append series mode" VALUE="Series number" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filename suffix" NICKNAME="Add filename suffix" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File format" NICKNAME="File format" VALUE="TIF" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save as RGB" NICKNAME="Save as RGB" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Compression mode" NICKNAME="Compression mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quality (0-100)" NICKNAME="Quality (0-100)" VALUE="100" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame rate (fps)" NICKNAME="Frame rate (fps)" VALUE="25" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Flatten overlay" NICKNAME="Flatten overlay" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;/ROOT&gt;</t>
+          <t xml:space="preserve"> image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement to filter on" NICKNAME="Measurement to filter on" VALUE="SHAPE // VOLUME_(µm³)" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962497111" NAME="GUI separator" NICKNAME="Measurements" NOTES="Modules in this section are involved with additional measurements assigned to the detectetd nuclei." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.intensity.MeasureObjectIntensity" DISABLEABLE="false" ENABLED="true" ID="1636962461046" NAME="Measure object intensity" NICKNAME="Measure object intensity" NOTES="Measuring the intensity of the &amp;quot;Raw&amp;quot; image coincident with each &amp;quot;Nuclei&amp;quot; object.&amp;#10;&amp;#10;As with the &amp;quot;Measure object shape&amp;quot; module, this will make a separate measurement for each object in the collection.  In this case that measurement is the mean, min, max, sum and standard deviation of all pixel intensities coincident with the coordinates of each object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure weighted centre" NICKNAME="Measure weighted centre" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_MAX" NICKNAME="INTENSITY // Raw_MAX" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_MEAN" NICKNAME="INTENSITY // Raw_MEAN" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_MIN" NICKNAME="INTENSITY // Raw_MIN" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_STDEV" NICKNAME="INTENSITY // Raw_STDEV" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="INTENSITY // Raw_SUM" NICKNAME="INTENSITY // Raw_SUM" OBJECT_NAME="Nuclei"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.process.FitLongestChord" DISABLEABLE="false" ENABLED="true" ID="1690970094383" NAME="Fit longest chord" NICKNAME="Fit longest chord" NOTES="Measuring the &amp;quot;longest chord&amp;quot; for each nucleus.  The longest chord is the longest straight line that can be placed between any two points on the surface of an object.  In other words, it is the maximum diameter." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure object width" NICKNAME="Measure object width" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure object orientation" NICKNAME="Measure object orientation" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store end points" NICKNAME="Store end points" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="LONGEST_CHORD // LENGTH (PX)" NICKNAME="LONGEST_CHORD // LENGTH (PX)" OBJECT_NAME="Nuclei"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="LONGEST_CHORD // LENGTH (µm)" NICKNAME="LONGEST_CHORD // LENGTH (µm)" OBJECT_NAME="Nuclei"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1636962505950" NAME="GUI separator" NICKNAME="Image output" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectFill" DISABLEABLE="false" ENABLED="true" ID="1636962635839" NAME="Add object fill" NICKNAME="Add object fill" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Measurement value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="White" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="LONGEST_CHORD // LENGTH (µm)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="25" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Raw" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectOutline" DISABLEABLE="false" ENABLED="true" ID="1636962596250" NAME="Add object outline" NICKNAME="Add object outline" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.1"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="White" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reduce line complexity" NICKNAME="Reduce line complexity" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Line interpolation" NICKNAME="Line interpolation" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Line width" NICKNAME="Line width" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddLabels" DISABLEABLE="false" ENABLED="true" ID="1690970140097" NAME="Add labels" NICKNAME="Add labels" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="White" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Nuclei" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Label mode" NICKNAME="Label mode" VALUE="ID" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Decimal places" NICKNAME="Decimal places" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use scientific notation" NICKNAME="Use scientific notation" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Label size" NICKNAME="Label size" VALUE="10" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X-offset" NICKNAME="X-offset" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y-offset" NICKNAME="Y-offset" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Centre text" NICKNAME="Centre text" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for label" NICKNAME="Child objects for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for label" NICKNAME="Parent object for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for label" NICKNAME="Partner objects for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for label" NICKNAME="Measurement for label" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Prefix" NICKNAME="Prefix" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Suffix" NICKNAME="Suffix" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Label position" NICKNAME="Label position" VALUE="Centre of object" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X-position measurement" NICKNAME="X-position measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y-position measurement" NICKNAME="Y-position measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z-position measurement" NICKNAME="Z-position measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X-position" NICKNAME="X-position" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y-position" NICKNAME="Y-position" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z-position" NICKNAME="Z-position" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all object slices" NICKNAME="Render in all object slices" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.ShowImage" DISABLEABLE="true" ENABLED="false" ID="1636962716078" NAME="Show image" NICKNAME="Show image" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="true" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Display image" NICKNAME="Display image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Title mode" NICKNAME="Title mode" VALUE="Image name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quick normalisation" NICKNAME="Quick normalisation" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageSaver" DISABLEABLE="true" ENABLED="true" ID="1636962735245" NAME="Save image" NICKNAME="Save image" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Save location" NICKNAME="Save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name (generic)" NICKNAME="File name (generic)" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append series mode" NICKNAME="Append series mode" VALUE="Series number" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filename suffix" NICKNAME="Add filename suffix" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File format" NICKNAME="File format" VALUE="TIF" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save as RGB" NICKNAME="Save as RGB" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Compression mode" NICKNAME="Compression mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quality (0-100)" NICKNAME="Quality (0-100)" VALUE="100" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame rate (fps)" NICKNAME="Frame rate (fps)" VALUE="25" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Flatten overlay" NICKNAME="Flatten overlay" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;/ROOT&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>